<commit_message>
demand weights file updated
</commit_message>
<xml_diff>
--- a/data/input/tom_demand_setup.xlsx
+++ b/data/input/tom_demand_setup.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac1445618/Library/CloudStorage/GoogleDrive-ruipedrosaraiva@gmail.com/My Drive/dev/python/ctt/tom_demand/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F04BA5-2935-7F4D-87E9-23811292BB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1923FE-2C35-6643-AEED-54DB84B7EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="2" xr2:uid="{9D2BC160-0631-EE46-87AB-AABB69ACE5D9}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{9D2BC160-0631-EE46-87AB-AABB69ACE5D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="weights_ra" sheetId="2" r:id="rId1"/>
+    <sheet name="DEMAND WEIGHTS" sheetId="4" r:id="rId1"/>
     <sheet name="weights_rs" sheetId="1" r:id="rId2"/>
-    <sheet name="ideas" sheetId="3" r:id="rId3"/>
+    <sheet name="weights_ra" sheetId="2" r:id="rId3"/>
+    <sheet name="ideas" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ideas!$A$1:$J$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">weights_ra!$A$1:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ideas!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">weights_ra!$A$1:$D$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="131">
   <si>
     <t>RevenueStream</t>
   </si>
@@ -301,13 +302,172 @@
   </si>
   <si>
     <t>_RA</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>CSI</t>
+  </si>
+  <si>
+    <t>CTTE</t>
+  </si>
+  <si>
+    <t>ECM</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>OPERATIONS</t>
+  </si>
+  <si>
+    <t>ACR</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>AVC</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>GFC</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>DPO</t>
+  </si>
+  <si>
+    <t>SSJ</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>CORPORATE</t>
+  </si>
+  <si>
+    <t>SI-PRD</t>
+  </si>
+  <si>
+    <t>SI-OPS</t>
+  </si>
+  <si>
+    <t>SI-CRP</t>
+  </si>
+  <si>
+    <t>TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>DAT</t>
+  </si>
+  <si>
+    <t>eCOMMERCE</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
+    <t>CMO</t>
+  </si>
+  <si>
+    <t>CCO</t>
+  </si>
+  <si>
+    <t>ATC</t>
+  </si>
+  <si>
+    <t>IDC</t>
+  </si>
+  <si>
+    <t>CFO</t>
+  </si>
+  <si>
+    <t>CIO</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>CHR</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>Data &amp; AI</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>operations</t>
+  </si>
+  <si>
+    <t>corporate</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>PORTUGAL</t>
+  </si>
+  <si>
+    <t>ESPAÑA</t>
+  </si>
+  <si>
+    <t>DEMAND 2025</t>
+  </si>
+  <si>
+    <t>DEMAND 2026</t>
+  </si>
+  <si>
+    <t>MAIL</t>
+  </si>
+  <si>
+    <t>FULFILMENT</t>
+  </si>
+  <si>
+    <t>PAYMENTS</t>
+  </si>
+  <si>
+    <t>RETAIL &amp; FINANCIAL SERVICES</t>
+  </si>
+  <si>
+    <t>BUSINESS SOLUTIONS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,8 +514,33 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +559,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -384,10 +581,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -398,11 +596,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent 2" xfId="1" xr:uid="{B4B05582-F7D3-F142-B20F-B4C84A0F58E6}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -420,6 +648,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -792,28 +1090,3493 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D521F980-2E5F-EC49-B62F-4F6A4A27A40F}">
-  <dimension ref="A1:O61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB758DFD-45B9-6B4E-99A1-FC80C2C804E6}">
+  <dimension ref="A1:AF88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AA46" sqref="AA46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.83203125" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.83203125" customWidth="1"/>
+    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+    </row>
+    <row r="3" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0.38</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.19</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="13">
+        <v>0.19</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" s="13">
+        <v>0.19</v>
+      </c>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="R3" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="X5" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="Z5" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="AA5" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="AD5" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AE5" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="AF5" s="14">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="12"/>
+      <c r="AF9" s="12"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J14" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="12"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="18">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="12"/>
+      <c r="AC18" s="12"/>
+      <c r="AD18" s="12"/>
+      <c r="AE18" s="12"/>
+      <c r="AF18" s="12"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="17">
+        <f>VLOOKUP(A21,weights_rs!$A:$B,2,FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="C21" s="7" t="b">
+        <f>(B23+F23+J23+N23+R23+V23)=100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="b">
+        <f>B23=SUM(B24:B32)</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="7" t="b">
+        <f>F23=SUM(F24:F32)</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="7" t="b">
+        <f>J23=SUM(J24:J32)</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" s="7" t="b">
+        <f>N23=SUM(N24:N32)</f>
+        <v>1</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="7" t="b">
+        <f>R23=SUM(R24:R32)</f>
+        <v>1</v>
+      </c>
+      <c r="U22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V22" s="7" t="b">
+        <f>V23=SUM(V24:V32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="13">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <f>B23*($B$21/100)</f>
+        <v>12.5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="13">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1">
+        <f>F23*($B$21/100)</f>
+        <v>12.5</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="13">
+        <v>20</v>
+      </c>
+      <c r="K23" s="1">
+        <f>J23*($B$21/100)</f>
+        <v>10</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" s="13">
+        <v>20</v>
+      </c>
+      <c r="O23" s="1">
+        <f>N23*($B$21/100)</f>
+        <v>10</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R23" s="13">
+        <v>5</v>
+      </c>
+      <c r="S23" s="1">
+        <f>R23*($B$21/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V23" s="13">
+        <v>5</v>
+      </c>
+      <c r="W23" s="1">
+        <f>V23*($B$21/100)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="12">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:C31" si="0">B24*($B$21/100)</f>
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="12">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G31" si="1">F24*($B$21/100)</f>
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="12">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" ref="K24:K31" si="2">J24*($B$21/100)</f>
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>113</v>
+      </c>
+      <c r="N24" s="12">
+        <v>20</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" ref="O24:O31" si="3">N24*($B$21/100)</f>
+        <v>10</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" s="12">
+        <v>5</v>
+      </c>
+      <c r="S24" s="1">
+        <f t="shared" ref="S24:S31" si="4">R24*($B$21/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="U24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V24" s="12">
+        <v>5</v>
+      </c>
+      <c r="W24" s="1">
+        <f t="shared" ref="W24:W31" si="5">V24*($B$21/100)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="12">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="12">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" s="12">
+        <v>8</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N25" s="12"/>
+      <c r="O25" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="12"/>
+      <c r="S25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="12"/>
+      <c r="W25" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="12">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="12">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>114</v>
+      </c>
+      <c r="J26" s="12">
+        <v>2</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N26" s="12"/>
+      <c r="O26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="12"/>
+      <c r="S26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="12"/>
+      <c r="W26" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="12">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" s="12">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="N27" s="12"/>
+      <c r="O27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="12"/>
+      <c r="S27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="12"/>
+      <c r="W27" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="12">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>116</v>
+      </c>
+      <c r="J28" s="12">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="N28" s="12"/>
+      <c r="O28" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="12"/>
+      <c r="S28" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="12"/>
+      <c r="W28" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="12"/>
+      <c r="O29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="12"/>
+      <c r="S29" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="12"/>
+      <c r="W29" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="12">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="K30" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="12"/>
+      <c r="O30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="12"/>
+      <c r="S30" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="12"/>
+      <c r="W30" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="12">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="12"/>
+      <c r="K31" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="12"/>
+      <c r="O31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R31" s="12"/>
+      <c r="S31" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V31" s="12"/>
+      <c r="W31" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="17">
+        <f>VLOOKUP(A34,weights_rs!$A:$B,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="C34" s="7" t="b">
+        <f>(B36+F36+J36+N36+R36+V36)=100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="7" t="b">
+        <f>B36=SUM(B37:B52)</f>
+        <v>1</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="7" t="b">
+        <f>F36=SUM(F37:F52)</f>
+        <v>1</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="7" t="b">
+        <f>J36=SUM(J37:J52)</f>
+        <v>1</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N35" s="7" t="b">
+        <f>N36=SUM(N37:N52)</f>
+        <v>1</v>
+      </c>
+      <c r="Q35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R35" s="7" t="b">
+        <f>R36=SUM(R37:R52)</f>
+        <v>1</v>
+      </c>
+      <c r="U35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V35" s="7" t="b">
+        <f>V36=SUM(V37:V52)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1">
+        <f>B36*($B$34/100)</f>
+        <v>6.25</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1">
+        <v>25</v>
+      </c>
+      <c r="G36" s="1">
+        <f>F36*($B$34/100)</f>
+        <v>6.25</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="1">
+        <v>20</v>
+      </c>
+      <c r="K36" s="1">
+        <f>J36*($B$34/100)</f>
+        <v>5</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N36" s="1">
+        <v>20</v>
+      </c>
+      <c r="O36" s="1">
+        <f>N36*($B$34/100)</f>
+        <v>5</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R36" s="1">
+        <v>5</v>
+      </c>
+      <c r="S36" s="1">
+        <f>R36*($B$34/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V36" s="1">
+        <v>5</v>
+      </c>
+      <c r="W36" s="1">
+        <f>V36*($B$34/100)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ref="C37:C51" si="6">B37*($B$34/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" ref="G37:G51" si="7">F37*($B$34/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" ref="K37:K51" si="8">J37*($B$34/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37">
+        <v>10</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" ref="O37:O51" si="9">N37*($B$34/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>14</v>
+      </c>
+      <c r="R37">
+        <v>5</v>
+      </c>
+      <c r="S37" s="1">
+        <f t="shared" ref="S37:S51" si="10">R37*($B$34/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="U37" t="s">
+        <v>12</v>
+      </c>
+      <c r="V37">
+        <v>5</v>
+      </c>
+      <c r="W37" s="1">
+        <f t="shared" ref="W37:W51" si="11">V37*($B$34/100)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="M38" t="s">
+        <v>75</v>
+      </c>
+      <c r="N38">
+        <v>10</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="9"/>
+        <v>2.5</v>
+      </c>
+      <c r="S38" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="I39" t="s">
+        <v>88</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S39" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S40" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W40" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>76</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S41" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W41" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>90</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W42" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C43" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>91</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S43" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W43" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C44" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>92</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S44" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W44" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C45" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>93</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S45" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W45" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C46" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>94</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O46" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S46" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W46" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C47" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>95</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O47" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S47" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W47" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C48" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>96</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O48" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S48" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W48" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C49" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>97</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O49" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S49" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W49" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C50" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>98</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O50" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W50" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C51" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>99</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="O51" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S51" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W51" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="12"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="17">
+        <f>VLOOKUP(A54,weights_rs!$A:$B,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="C54" s="7" t="b">
+        <f>(B56+F56+J56+N56+R56+V56)=100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="7" t="b">
+        <f>B56=SUM(B57:B61)</f>
+        <v>1</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="7" t="b">
+        <f>F56=SUM(F57:F61)</f>
+        <v>1</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" s="7" t="b">
+        <f>J56=SUM(J57:J61)</f>
+        <v>1</v>
+      </c>
+      <c r="M55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N55" s="7" t="b">
+        <f>N56=SUM(N57:N61)</f>
+        <v>1</v>
+      </c>
+      <c r="Q55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R55" s="7" t="b">
+        <f>R56=SUM(R57:R61)</f>
+        <v>1</v>
+      </c>
+      <c r="U55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V55" s="7" t="b">
+        <f>V56=SUM(V57:V61)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1">
+        <f>B56*($B$54/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1">
+        <v>25</v>
+      </c>
+      <c r="G56" s="1">
+        <f>F56*($B$54/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" s="1">
+        <v>20</v>
+      </c>
+      <c r="K56" s="1">
+        <f>J56*($B$54/100)</f>
+        <v>2</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N56" s="1">
+        <v>20</v>
+      </c>
+      <c r="O56" s="1">
+        <f>N56*($B$54/100)</f>
+        <v>2</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R56" s="1">
+        <v>5</v>
+      </c>
+      <c r="S56" s="1">
+        <f>R56*($B$54/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="U56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V56" s="1">
+        <v>5</v>
+      </c>
+      <c r="W56" s="1">
+        <f>V56*($B$54/100)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57">
+        <v>19</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" ref="C57:C60" si="12">B57*($B$54/100)</f>
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" ref="G57:G60" si="13">F57*($B$54/100)</f>
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
+        <v>23</v>
+      </c>
+      <c r="J57">
+        <v>20</v>
+      </c>
+      <c r="K57" s="1">
+        <f t="shared" ref="K57:K60" si="14">J57*($B$54/100)</f>
+        <v>2</v>
+      </c>
+      <c r="M57" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57">
+        <v>20</v>
+      </c>
+      <c r="O57" s="1">
+        <f t="shared" ref="O57:O60" si="15">N57*($B$54/100)</f>
+        <v>2</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>14</v>
+      </c>
+      <c r="R57">
+        <v>5</v>
+      </c>
+      <c r="S57" s="1">
+        <f t="shared" ref="S57:S60" si="16">R57*($B$54/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="U57" t="s">
+        <v>12</v>
+      </c>
+      <c r="V57">
+        <v>5</v>
+      </c>
+      <c r="W57" s="1">
+        <f t="shared" ref="W57:W60" si="17">V57*($B$54/100)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58">
+        <v>10</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K58" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O58" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="S58" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W58" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F59">
+        <v>5</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="K59" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O59" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="S59" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W59" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" s="1">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K60" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O60" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="S60" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W60" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12"/>
+      <c r="R61" s="12"/>
+      <c r="S61" s="12"/>
+      <c r="T61" s="12"/>
+      <c r="U61" s="12"/>
+      <c r="V61" s="12"/>
+      <c r="W61" s="12"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="17">
+        <f>VLOOKUP(A63,weights_rs!$A:$B,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="C63" s="7" t="b">
+        <f>(B65+F65+J65+N65+R65+V65)=100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="7" t="b">
+        <f>B65=SUM(B66:B70)</f>
+        <v>1</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="7" t="b">
+        <f>F65=SUM(F66:F70)</f>
+        <v>1</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J64" s="7" t="b">
+        <f>J65=SUM(J66:J70)</f>
+        <v>1</v>
+      </c>
+      <c r="M64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N64" s="7" t="b">
+        <f>N65=SUM(N66:N70)</f>
+        <v>1</v>
+      </c>
+      <c r="Q64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R64" s="7" t="b">
+        <f>R65=SUM(R66:R70)</f>
+        <v>1</v>
+      </c>
+      <c r="U64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V64" s="7" t="b">
+        <f>V65=SUM(V66:V70)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="1">
+        <v>25</v>
+      </c>
+      <c r="C65" s="1">
+        <f>B65*($B$63/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="1">
+        <v>25</v>
+      </c>
+      <c r="G65" s="1">
+        <f>F65*($B$63/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" s="1">
+        <v>20</v>
+      </c>
+      <c r="K65" s="1">
+        <f>J65*($B$63/100)</f>
+        <v>1</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N65" s="1">
+        <v>20</v>
+      </c>
+      <c r="O65" s="1">
+        <f>N65*($B$63/100)</f>
+        <v>1</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R65" s="1">
+        <v>5</v>
+      </c>
+      <c r="S65" s="1">
+        <f>R65*($B$63/100)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V65" s="1">
+        <v>5</v>
+      </c>
+      <c r="W65" s="1">
+        <f>V65*($B$63/100)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66">
+        <v>19</v>
+      </c>
+      <c r="C66" s="1">
+        <f t="shared" ref="C66:C69" si="18">B66*($B$63/100)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66">
+        <v>10</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" ref="G66:G69" si="19">F66*($B$63/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>23</v>
+      </c>
+      <c r="J66">
+        <v>20</v>
+      </c>
+      <c r="K66" s="1">
+        <f t="shared" ref="K66:K69" si="20">J66*($B$63/100)</f>
+        <v>1</v>
+      </c>
+      <c r="M66" t="s">
+        <v>10</v>
+      </c>
+      <c r="N66">
+        <v>20</v>
+      </c>
+      <c r="O66" s="1">
+        <f t="shared" ref="O66:O69" si="21">N66*($B$63/100)</f>
+        <v>1</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>14</v>
+      </c>
+      <c r="R66">
+        <v>5</v>
+      </c>
+      <c r="S66" s="1">
+        <f t="shared" ref="S66:S69" si="22">R66*($B$63/100)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U66" t="s">
+        <v>12</v>
+      </c>
+      <c r="V66">
+        <v>5</v>
+      </c>
+      <c r="W66" s="1">
+        <f t="shared" ref="W66:W69" si="23">V66*($B$63/100)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" si="18"/>
+        <v>0.1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>27</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="19"/>
+        <v>0.5</v>
+      </c>
+      <c r="K67" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O67" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S67" s="1">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="W67" s="1">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" s="1">
+        <f t="shared" si="18"/>
+        <v>0.1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>85</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="19"/>
+        <v>0.25</v>
+      </c>
+      <c r="K68" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O68" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S68" s="1">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="W68" s="1">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" si="18"/>
+        <v>0.1</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K69" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O69" s="1">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S69" s="1">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="W69" s="1">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+      <c r="R70" s="12"/>
+      <c r="S70" s="12"/>
+      <c r="T70" s="12"/>
+      <c r="U70" s="12"/>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="17">
+        <f>VLOOKUP(A72,weights_rs!$A:$B,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="C72" s="7" t="b">
+        <f>(B74+F74+J74+N74+R74+V74)=100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" s="7" t="b">
+        <f>B74=SUM(B75:B79)</f>
+        <v>1</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="7" t="b">
+        <f>F74=SUM(F75:F79)</f>
+        <v>1</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J73" s="7" t="b">
+        <f>J74=SUM(J75:J79)</f>
+        <v>1</v>
+      </c>
+      <c r="M73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N73" s="7" t="b">
+        <f>N74=SUM(N75:N79)</f>
+        <v>1</v>
+      </c>
+      <c r="Q73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R73" s="7" t="b">
+        <f>R74=SUM(R75:R79)</f>
+        <v>1</v>
+      </c>
+      <c r="U73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V73" s="7" t="b">
+        <f>V74=SUM(V75:V79)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="1">
+        <v>25</v>
+      </c>
+      <c r="C74" s="1">
+        <f>B74*($B$72/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="1">
+        <v>25</v>
+      </c>
+      <c r="G74" s="1">
+        <f>F74*($B$72/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" s="1">
+        <v>20</v>
+      </c>
+      <c r="K74" s="1">
+        <f>J74*($B$72/100)</f>
+        <v>1</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N74" s="1">
+        <v>20</v>
+      </c>
+      <c r="O74" s="1">
+        <f>N74*($B$72/100)</f>
+        <v>1</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R74" s="1">
+        <v>5</v>
+      </c>
+      <c r="S74" s="1">
+        <f>R74*($B$72/100)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V74" s="1">
+        <v>5</v>
+      </c>
+      <c r="W74" s="1">
+        <f>V74*($B$72/100)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75">
+        <v>19</v>
+      </c>
+      <c r="C75" s="1">
+        <f t="shared" ref="C75:C78" si="24">B75*($B$72/100)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75">
+        <v>10</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" ref="G75:G78" si="25">F75*($B$72/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I75" t="s">
+        <v>23</v>
+      </c>
+      <c r="J75">
+        <v>20</v>
+      </c>
+      <c r="K75" s="1">
+        <f t="shared" ref="K75:K78" si="26">J75*($B$72/100)</f>
+        <v>1</v>
+      </c>
+      <c r="M75" t="s">
+        <v>10</v>
+      </c>
+      <c r="N75">
+        <v>20</v>
+      </c>
+      <c r="O75" s="1">
+        <f t="shared" ref="O75:O78" si="27">N75*($B$72/100)</f>
+        <v>1</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>14</v>
+      </c>
+      <c r="R75">
+        <v>5</v>
+      </c>
+      <c r="S75" s="1">
+        <f t="shared" ref="S75:S78" si="28">R75*($B$72/100)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U75" t="s">
+        <v>12</v>
+      </c>
+      <c r="V75">
+        <v>5</v>
+      </c>
+      <c r="W75" s="1">
+        <f t="shared" ref="W75:W78" si="29">V75*($B$72/100)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" s="1">
+        <f t="shared" si="24"/>
+        <v>0.1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76">
+        <v>10</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="25"/>
+        <v>0.5</v>
+      </c>
+      <c r="K76" s="1">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="O76" s="1">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="S76" s="1">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="W76" s="1">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" s="1">
+        <f t="shared" si="24"/>
+        <v>0.1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>85</v>
+      </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="25"/>
+        <v>0.25</v>
+      </c>
+      <c r="K77" s="1">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="O77" s="1">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="S77" s="1">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="W77" s="1">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" s="1">
+        <f t="shared" si="24"/>
+        <v>0.1</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="K78" s="1">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="O78" s="1">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="S78" s="1">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="W78" s="1">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="12"/>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12"/>
+      <c r="P79" s="12"/>
+      <c r="Q79" s="12"/>
+      <c r="R79" s="12"/>
+      <c r="S79" s="12"/>
+      <c r="T79" s="12"/>
+      <c r="U79" s="12"/>
+      <c r="V79" s="12"/>
+      <c r="W79" s="12"/>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="17">
+        <f>VLOOKUP(A81,weights_rs!$A:$B,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="C81" s="7" t="b">
+        <f>(B83+F83+J83+N83+R83+V83)=100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" s="7" t="b">
+        <f>B83=SUM(B84:B88)</f>
+        <v>1</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82" s="7" t="b">
+        <f>F83=SUM(F84:F88)</f>
+        <v>1</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J82" s="7" t="b">
+        <f>J83=SUM(J84:J88)</f>
+        <v>1</v>
+      </c>
+      <c r="M82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N82" s="7" t="b">
+        <f>N83=SUM(N84:N88)</f>
+        <v>1</v>
+      </c>
+      <c r="Q82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R82" s="7" t="b">
+        <f>R83=SUM(R84:R88)</f>
+        <v>1</v>
+      </c>
+      <c r="U82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V82" s="7" t="b">
+        <f>V83=SUM(V84:V88)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="1">
+        <v>25</v>
+      </c>
+      <c r="C83" s="1">
+        <f>B83*($B$81/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="1">
+        <v>25</v>
+      </c>
+      <c r="G83" s="1">
+        <f>F83*($B$81/100)</f>
+        <v>1.25</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J83" s="1">
+        <v>20</v>
+      </c>
+      <c r="K83" s="1">
+        <f>J83*($B$81/100)</f>
+        <v>1</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N83" s="1">
+        <v>20</v>
+      </c>
+      <c r="O83" s="1">
+        <f>N83*($B$81/100)</f>
+        <v>1</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R83" s="1">
+        <v>5</v>
+      </c>
+      <c r="S83" s="1">
+        <f>R83*($B$81/100)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V83" s="1">
+        <v>5</v>
+      </c>
+      <c r="W83" s="1">
+        <f>V83*($B$81/100)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84">
+        <v>19</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" ref="C84:C87" si="30">B84*($B$81/100)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84">
+        <v>10</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" ref="G84:G87" si="31">F84*($B$81/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I84" t="s">
+        <v>23</v>
+      </c>
+      <c r="J84">
+        <v>20</v>
+      </c>
+      <c r="K84" s="1">
+        <f t="shared" ref="K84:K87" si="32">J84*($B$81/100)</f>
+        <v>1</v>
+      </c>
+      <c r="M84" t="s">
+        <v>10</v>
+      </c>
+      <c r="N84">
+        <v>20</v>
+      </c>
+      <c r="O84" s="1">
+        <f t="shared" ref="O84:O87" si="33">N84*($B$81/100)</f>
+        <v>1</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>14</v>
+      </c>
+      <c r="R84">
+        <v>5</v>
+      </c>
+      <c r="S84" s="1">
+        <f t="shared" ref="S84:S87" si="34">R84*($B$81/100)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U84" t="s">
+        <v>12</v>
+      </c>
+      <c r="V84">
+        <v>5</v>
+      </c>
+      <c r="W84" s="1">
+        <f t="shared" ref="W84:W87" si="35">V84*($B$81/100)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85" s="1">
+        <f t="shared" si="30"/>
+        <v>0.1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>27</v>
+      </c>
+      <c r="F85">
+        <v>10</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="31"/>
+        <v>0.5</v>
+      </c>
+      <c r="K85" s="1">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="O85" s="1">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S85" s="1">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="W85" s="1">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86" s="1">
+        <f t="shared" si="30"/>
+        <v>0.1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>85</v>
+      </c>
+      <c r="F86">
+        <v>5</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="31"/>
+        <v>0.25</v>
+      </c>
+      <c r="K86" s="1">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="O86" s="1">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S86" s="1">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="W86" s="1">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" s="1">
+        <f t="shared" si="30"/>
+        <v>0.1</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="K87" s="1">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="O87" s="1">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S87" s="1">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="W87" s="1">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+      <c r="L88" s="12"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+      <c r="O88" s="12"/>
+      <c r="P88" s="12"/>
+      <c r="Q88" s="12"/>
+      <c r="R88" s="12"/>
+      <c r="S88" s="12"/>
+      <c r="T88" s="12"/>
+      <c r="U88" s="12"/>
+      <c r="V88" s="12"/>
+      <c r="W88" s="12"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B22 F22 J22 N22 R22 V22 V35 R35 N35 J35 F35 B35 B64 F64 J64 N64 R64 V64 V73 R73 N73 J73 F73 B73 V82 R82 N82 J82 F82 B82">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C72">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C81">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55 F55 J55 N55 R55 V55">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B369EC55-B648-3A4C-A439-D742FEF9A099}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4">
+        <f>SUM(B3:B20)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>25</v>
+      </c>
+      <c r="C4" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D521F980-2E5F-EC49-B62F-4F6A4A27A40F}">
+  <dimension ref="A1:O61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="8"/>
+    <col min="7" max="7" width="6.5" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="8"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.83203125" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="8"/>
+    <col min="13" max="13" width="6.5" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1911,7 +5674,7 @@
   </sheetData>
   <autoFilter ref="A1:D26" xr:uid="{D521F980-2E5F-EC49-B62F-4F6A4A27A40F}"/>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1924,7 +5687,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1937,7 +5700,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1945,115 +5708,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B369EC55-B648-3A4C-A439-D742FEF9A099}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4">
-        <f>SUM(B:B)</f>
-        <v>100</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D437AB-C2CB-8D43-BD8D-11D3278E662B}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2757,12 +6418,12 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"ALERT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"ALERT"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added the feature to allow different methods per queue
</commit_message>
<xml_diff>
--- a/data/input/tom_demand_setup.xlsx
+++ b/data/input/tom_demand_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac1445618/Library/CloudStorage/GoogleDrive-ruipedrosaraiva@gmail.com/My Drive/dev/python/ctt/tom_demand/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B92738-ADD9-1D42-BC9B-A5C20665B69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCADAB6F-0FE9-9244-B69E-E05CFBD5FE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29840" windowHeight="18560" activeTab="3" xr2:uid="{9D2BC160-0631-EE46-87AB-AABB69ACE5D9}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="159">
   <si>
     <t>RevenueStream</t>
   </si>
@@ -494,6 +494,54 @@
   </si>
   <si>
     <t>Ready for Solution</t>
+  </si>
+  <si>
+    <t>IDEA021</t>
+  </si>
+  <si>
+    <t>IDEA022</t>
+  </si>
+  <si>
+    <t>IDEA023</t>
+  </si>
+  <si>
+    <t>IDEA024</t>
+  </si>
+  <si>
+    <t>System 1</t>
+  </si>
+  <si>
+    <t>System 2</t>
+  </si>
+  <si>
+    <t>System 3</t>
+  </si>
+  <si>
+    <t>System 4</t>
+  </si>
+  <si>
+    <t>IDEA025</t>
+  </si>
+  <si>
+    <t>System 5</t>
+  </si>
+  <si>
+    <t>IDEA026</t>
+  </si>
+  <si>
+    <t>System 6</t>
+  </si>
+  <si>
+    <t>IDEA027</t>
+  </si>
+  <si>
+    <t>System 7</t>
+  </si>
+  <si>
+    <t>IDEA028</t>
+  </si>
+  <si>
+    <t>System 8</t>
   </si>
 </sst>
 </file>
@@ -503,7 +551,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -574,6 +622,12 @@
       <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -5743,11 +5797,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D437AB-C2CB-8D43-BD8D-11D3278E662B}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5874,7 +5928,7 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N21" si="0">D3&amp;"-"&amp;C3</f>
+        <f t="shared" ref="N3:N22" si="0">D3&amp;"-"&amp;C3</f>
         <v>Mail-GP B2B</v>
       </c>
       <c r="O3" t="str">
@@ -6530,12 +6584,225 @@
         <v>ALERT</v>
       </c>
     </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="0"/>
+        <v>Mail-SI</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="3">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" s="3">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" s="3">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="3">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" s="3">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="3">
+        <v>11</v>
+      </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K21" xr:uid="{25D437AB-C2CB-8D43-BD8D-11D3278E662B}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K21">
-      <sortCondition ref="C1:C21"/>
+      <sortCondition ref="A1:A21"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="N1">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"ALERT"</formula>

</xml_diff>

<commit_message>
Update input data setup file
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/input/tom_demand_setup.xlsx
+++ b/data/input/tom_demand_setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac1445618/Library/CloudStorage/GoogleDrive-ruipedrosaraiva@gmail.com/My Drive/dev/python/ctt/tom_demand/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCADAB6F-0FE9-9244-B69E-E05CFBD5FE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659BB6B4-CFE7-CE49-9E73-B36DA9DDB380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29840" windowHeight="18560" activeTab="3" xr2:uid="{9D2BC160-0631-EE46-87AB-AABB69ACE5D9}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18560" xr2:uid="{9D2BC160-0631-EE46-87AB-AABB69ACE5D9}"/>
   </bookViews>
   <sheets>
     <sheet name="DEMAND WEIGHTS" sheetId="4" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="161">
   <si>
     <t>RevenueStream</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>System 8</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>FINAL LIST</t>
   </si>
 </sst>
 </file>
@@ -663,7 +669,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -702,6 +708,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,16 +1185,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB758DFD-45B9-6B4E-99A1-FC80C2C804E6}">
-  <dimension ref="A1:AF88"/>
+  <dimension ref="A1:AF91"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.83203125" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -1209,7 +1217,7 @@
     <col min="22" max="22" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10.1640625" bestFit="1" customWidth="1"/>
@@ -2138,9 +2146,13 @@
         <f>V23*($B$21/100)</f>
         <v>2.5</v>
       </c>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>108</v>
       </c>
       <c r="B24" s="12">
@@ -2180,7 +2192,7 @@
         <f t="shared" ref="O24:O31" si="3">N24*($B$21/100)</f>
         <v>10</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" s="19" t="s">
         <v>14</v>
       </c>
       <c r="R24" s="12">
@@ -2190,7 +2202,7 @@
         <f t="shared" ref="S24:S31" si="4">R24*($B$21/100)</f>
         <v>2.5</v>
       </c>
-      <c r="U24" t="s">
+      <c r="U24" s="19" t="s">
         <v>12</v>
       </c>
       <c r="V24" s="12">
@@ -2202,7 +2214,7 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="20" t="s">
         <v>109</v>
       </c>
       <c r="B25" s="12">
@@ -2212,7 +2224,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="19" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="12">
@@ -2249,7 +2261,7 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="20" t="s">
         <v>111</v>
       </c>
       <c r="B26" s="12">
@@ -2296,7 +2308,7 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="12">
@@ -2385,7 +2397,7 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B29" s="12">
@@ -2640,7 +2652,7 @@
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B37">
@@ -2650,7 +2662,7 @@
         <f t="shared" ref="C37:C51" si="6">B37*($B$34/100)</f>
         <v>1.25</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="19" t="s">
         <v>8</v>
       </c>
       <c r="F37">
@@ -2660,7 +2672,7 @@
         <f t="shared" ref="G37:G51" si="7">F37*($B$34/100)</f>
         <v>2.5</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="19" t="s">
         <v>87</v>
       </c>
       <c r="J37">
@@ -2670,7 +2682,7 @@
         <f t="shared" ref="K37:K51" si="8">J37*($B$34/100)</f>
         <v>0.5</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M37" s="19" t="s">
         <v>10</v>
       </c>
       <c r="N37">
@@ -2680,7 +2692,7 @@
         <f t="shared" ref="O37:O51" si="9">N37*($B$34/100)</f>
         <v>2.5</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="Q37" s="19" t="s">
         <v>14</v>
       </c>
       <c r="R37">
@@ -2690,7 +2702,7 @@
         <f t="shared" ref="S37:S51" si="10">R37*($B$34/100)</f>
         <v>1.25</v>
       </c>
-      <c r="U37" t="s">
+      <c r="U37" s="19" t="s">
         <v>12</v>
       </c>
       <c r="V37">
@@ -2712,7 +2724,7 @@
         <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="19" t="s">
         <v>27</v>
       </c>
       <c r="F38">
@@ -2732,7 +2744,7 @@
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="19" t="s">
         <v>75</v>
       </c>
       <c r="N38">
@@ -2752,7 +2764,7 @@
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B39">
@@ -2810,7 +2822,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="19" t="s">
         <v>89</v>
       </c>
       <c r="J40">
@@ -2848,7 +2860,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="19" t="s">
         <v>76</v>
       </c>
       <c r="J41">
@@ -2880,7 +2892,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="19" t="s">
         <v>90</v>
       </c>
       <c r="J42">
@@ -3072,7 +3084,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="19" t="s">
         <v>96</v>
       </c>
       <c r="J48">
@@ -3168,8 +3180,8 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I51" t="s">
-        <v>99</v>
+      <c r="I51" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="J51">
         <v>1</v>
@@ -3278,41 +3290,41 @@
         <v>5</v>
       </c>
       <c r="B56" s="1">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="C56" s="1">
-        <f>B56*($B$54/100)</f>
-        <v>2.5</v>
+        <f>B56*($B$72/100)</f>
+        <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F56" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G56" s="1">
-        <f>F56*($B$54/100)</f>
-        <v>2.5</v>
+        <f>F56*($B$72/100)</f>
+        <v>0</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K56" s="1">
-        <f>J56*($B$54/100)</f>
-        <v>2</v>
+        <f>J56*($B$72/100)</f>
+        <v>0</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N56" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O56" s="1">
-        <f>N56*($B$54/100)</f>
-        <v>2</v>
+        <f>N56*($B$72/100)</f>
+        <v>0.5</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>117</v>
@@ -3321,8 +3333,8 @@
         <v>5</v>
       </c>
       <c r="S56" s="1">
-        <f>R56*($B$54/100)</f>
-        <v>0.5</v>
+        <f>R56*($B$72/100)</f>
+        <v>0.25</v>
       </c>
       <c r="U56" s="1" t="s">
         <v>12</v>
@@ -3331,50 +3343,41 @@
         <v>5</v>
       </c>
       <c r="W56" s="1">
-        <f>V56*($B$54/100)</f>
-        <v>0.5</v>
+        <f>V56*($B$72/100)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>24</v>
+      <c r="A57" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" ref="C57:C60" si="12">B57*($B$54/100)</f>
-        <v>1.9000000000000001</v>
-      </c>
-      <c r="E57" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57">
-        <v>10</v>
+        <f t="shared" ref="C57" si="12">B57*($B$72/100)</f>
+        <v>4</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" ref="G57:G60" si="13">F57*($B$54/100)</f>
-        <v>1</v>
-      </c>
-      <c r="I57" t="s">
-        <v>23</v>
+        <f t="shared" ref="G57" si="13">F57*($B$72/100)</f>
+        <v>0</v>
       </c>
       <c r="J57">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" ref="K57:K60" si="14">J57*($B$54/100)</f>
-        <v>2</v>
+        <f t="shared" ref="K57" si="14">J57*($B$72/100)</f>
+        <v>0</v>
       </c>
       <c r="M57" t="s">
         <v>10</v>
       </c>
       <c r="N57">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" ref="O57:O60" si="15">N57*($B$54/100)</f>
-        <v>2</v>
+        <f t="shared" ref="O57" si="15">N57*($B$72/100)</f>
+        <v>0.5</v>
       </c>
       <c r="Q57" t="s">
         <v>14</v>
@@ -3383,8 +3386,8 @@
         <v>5</v>
       </c>
       <c r="S57" s="1">
-        <f t="shared" ref="S57:S60" si="16">R57*($B$54/100)</f>
-        <v>0.5</v>
+        <f t="shared" ref="S57" si="16">R57*($B$72/100)</f>
+        <v>0.25</v>
       </c>
       <c r="U57" t="s">
         <v>12</v>
@@ -3393,115 +3396,85 @@
         <v>5</v>
       </c>
       <c r="W57" s="1">
-        <f t="shared" ref="W57:W60" si="17">V57*($B$54/100)</f>
-        <v>0.5</v>
+        <f t="shared" ref="W57" si="17">V57*($B$72/100)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58">
-        <v>2</v>
-      </c>
       <c r="C58" s="1">
-        <f t="shared" si="12"/>
-        <v>0.2</v>
-      </c>
-      <c r="E58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58">
-        <v>10</v>
+        <f t="shared" ref="C58:C60" si="18">B58*($B$54/100)</f>
+        <v>0</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="13"/>
-        <v>1</v>
+        <f t="shared" ref="G58:G60" si="19">F58*($B$54/100)</f>
+        <v>0</v>
       </c>
       <c r="K58" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="K58:K60" si="20">J58*($B$54/100)</f>
         <v>0</v>
       </c>
       <c r="O58" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="O58:O60" si="21">N58*($B$54/100)</f>
         <v>0</v>
       </c>
       <c r="S58" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="S58:S60" si="22">R58*($B$54/100)</f>
         <v>0</v>
       </c>
       <c r="W58" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="W58:W60" si="23">V58*($B$54/100)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59">
-        <v>2</v>
-      </c>
       <c r="C59" s="1">
-        <f t="shared" si="12"/>
-        <v>0.2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>85</v>
-      </c>
-      <c r="F59">
-        <v>5</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
       <c r="K59" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O59" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W59" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60">
-        <v>2</v>
-      </c>
       <c r="C60" s="1">
-        <f t="shared" si="12"/>
-        <v>0.2</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K60" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O60" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S60" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W60" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -3592,11 +3565,11 @@
         <v>5</v>
       </c>
       <c r="B65" s="1">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C65" s="1">
         <f>B65*($B$63/100)</f>
-        <v>1.25</v>
+        <v>2.25</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>7</v>
@@ -3612,11 +3585,11 @@
         <v>13</v>
       </c>
       <c r="J65" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K65" s="1">
         <f>J65*($B$63/100)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>9</v>
@@ -3650,35 +3623,29 @@
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B66">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" ref="C66:C69" si="18">B66*($B$63/100)</f>
-        <v>0.95000000000000007</v>
+        <f t="shared" ref="C66:C69" si="24">B66*($B$63/100)</f>
+        <v>2.25</v>
       </c>
       <c r="E66" t="s">
         <v>8</v>
       </c>
       <c r="F66">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" ref="G66:G69" si="19">F66*($B$63/100)</f>
-        <v>0.5</v>
-      </c>
-      <c r="I66" t="s">
-        <v>23</v>
-      </c>
-      <c r="J66">
-        <v>20</v>
+        <f t="shared" ref="G66:G69" si="25">F66*($B$63/100)</f>
+        <v>0.65</v>
       </c>
       <c r="K66" s="1">
-        <f t="shared" ref="K66:K69" si="20">J66*($B$63/100)</f>
-        <v>1</v>
+        <f t="shared" ref="K66:K69" si="26">J66*($B$63/100)</f>
+        <v>0</v>
       </c>
       <c r="M66" t="s">
         <v>10</v>
@@ -3687,7 +3654,7 @@
         <v>20</v>
       </c>
       <c r="O66" s="1">
-        <f t="shared" ref="O66:O69" si="21">N66*($B$63/100)</f>
+        <f t="shared" ref="O66:O69" si="27">N66*($B$63/100)</f>
         <v>1</v>
       </c>
       <c r="Q66" t="s">
@@ -3697,7 +3664,7 @@
         <v>5</v>
       </c>
       <c r="S66" s="1">
-        <f t="shared" ref="S66:S69" si="22">R66*($B$63/100)</f>
+        <f t="shared" ref="S66:S69" si="28">R66*($B$63/100)</f>
         <v>0.25</v>
       </c>
       <c r="U66" t="s">
@@ -3707,115 +3674,91 @@
         <v>5</v>
       </c>
       <c r="W66" s="1">
-        <f t="shared" ref="W66:W69" si="23">V66*($B$63/100)</f>
+        <f t="shared" ref="W66:W69" si="29">V66*($B$63/100)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67">
-        <v>2</v>
-      </c>
       <c r="C67" s="1">
-        <f t="shared" si="18"/>
-        <v>0.1</v>
+        <f t="shared" si="24"/>
+        <v>0</v>
       </c>
       <c r="E67" t="s">
         <v>27</v>
       </c>
       <c r="F67">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" si="19"/>
-        <v>0.5</v>
+        <f t="shared" si="25"/>
+        <v>0.60000000000000009</v>
       </c>
       <c r="K67" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W67" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68">
-        <v>2</v>
-      </c>
       <c r="C68" s="1">
-        <f t="shared" si="18"/>
-        <v>0.1</v>
-      </c>
-      <c r="E68" t="s">
-        <v>85</v>
-      </c>
-      <c r="F68">
-        <v>5</v>
+        <f t="shared" si="24"/>
+        <v>0</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" si="19"/>
-        <v>0.25</v>
+        <f t="shared" si="25"/>
+        <v>0</v>
       </c>
       <c r="K68" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O68" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="S68" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W68" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69">
-        <v>2</v>
-      </c>
       <c r="C69" s="1">
-        <f t="shared" si="18"/>
-        <v>0.1</v>
+        <f t="shared" si="24"/>
+        <v>0</v>
       </c>
       <c r="G69" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K69" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O69" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="S69" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W69" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -3906,41 +3849,41 @@
         <v>5</v>
       </c>
       <c r="B74" s="1">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="C74" s="1">
         <f>B74*($B$72/100)</f>
-        <v>1.25</v>
+        <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F74" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G74" s="1">
         <f>F74*($B$72/100)</f>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J74" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K74" s="1">
         <f>J74*($B$72/100)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N74" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O74" s="1">
         <f>N74*($B$72/100)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q74" s="1" t="s">
         <v>117</v>
@@ -3964,45 +3907,36 @@
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="A75" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" ref="C75:C78" si="24">B75*($B$72/100)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="E75" t="s">
-        <v>8</v>
-      </c>
-      <c r="F75">
-        <v>10</v>
+        <f t="shared" ref="C75:C78" si="30">B75*($B$72/100)</f>
+        <v>4</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" ref="G75:G78" si="25">F75*($B$72/100)</f>
-        <v>0.5</v>
-      </c>
-      <c r="I75" t="s">
-        <v>23</v>
+        <f t="shared" ref="G75:G78" si="31">F75*($B$72/100)</f>
+        <v>0</v>
       </c>
       <c r="J75">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K75" s="1">
-        <f t="shared" ref="K75:K78" si="26">J75*($B$72/100)</f>
-        <v>1</v>
+        <f t="shared" ref="K75:K78" si="32">J75*($B$72/100)</f>
+        <v>0</v>
       </c>
       <c r="M75" t="s">
         <v>10</v>
       </c>
       <c r="N75">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O75" s="1">
-        <f t="shared" ref="O75:O78" si="27">N75*($B$72/100)</f>
-        <v>1</v>
+        <f t="shared" ref="O75:O78" si="33">N75*($B$72/100)</f>
+        <v>0.5</v>
       </c>
       <c r="Q75" t="s">
         <v>14</v>
@@ -4011,7 +3945,7 @@
         <v>5</v>
       </c>
       <c r="S75" s="1">
-        <f t="shared" ref="S75:S78" si="28">R75*($B$72/100)</f>
+        <f t="shared" ref="S75:S78" si="34">R75*($B$72/100)</f>
         <v>0.25</v>
       </c>
       <c r="U75" t="s">
@@ -4021,115 +3955,85 @@
         <v>5</v>
       </c>
       <c r="W75" s="1">
-        <f t="shared" ref="W75:W78" si="29">V75*($B$72/100)</f>
+        <f t="shared" ref="W75:W78" si="35">V75*($B$72/100)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>79</v>
-      </c>
-      <c r="B76">
-        <v>2</v>
-      </c>
       <c r="C76" s="1">
-        <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="E76" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76">
-        <v>10</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="25"/>
-        <v>0.5</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="K76" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O76" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S76" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W76" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77">
-        <v>2</v>
-      </c>
       <c r="C77" s="1">
-        <f t="shared" si="24"/>
-        <v>0.1</v>
-      </c>
-      <c r="E77" t="s">
-        <v>85</v>
-      </c>
-      <c r="F77">
-        <v>5</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="25"/>
-        <v>0.25</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="K77" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S77" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W77" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78">
-        <v>2</v>
-      </c>
       <c r="C78" s="1">
-        <f t="shared" si="24"/>
-        <v>0.1</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="K78" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O78" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="S78" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W78" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
     </row>
@@ -4220,21 +4124,21 @@
         <v>5</v>
       </c>
       <c r="B83" s="1">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C83" s="1">
         <f>B83*($B$81/100)</f>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F83" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G83" s="1">
         <f>F83*($B$81/100)</f>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>13</v>
@@ -4278,25 +4182,19 @@
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="A84" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B84">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" ref="C84:C87" si="30">B84*($B$81/100)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="E84" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84">
-        <v>10</v>
+        <f t="shared" ref="C84:C87" si="36">B84*($B$81/100)</f>
+        <v>1.25</v>
       </c>
       <c r="G84" s="1">
-        <f t="shared" ref="G84:G87" si="31">F84*($B$81/100)</f>
-        <v>0.5</v>
+        <f t="shared" ref="G84:G87" si="37">F84*($B$81/100)</f>
+        <v>0</v>
       </c>
       <c r="I84" t="s">
         <v>23</v>
@@ -4305,7 +4203,7 @@
         <v>20</v>
       </c>
       <c r="K84" s="1">
-        <f t="shared" ref="K84:K87" si="32">J84*($B$81/100)</f>
+        <f t="shared" ref="K84:K87" si="38">J84*($B$81/100)</f>
         <v>1</v>
       </c>
       <c r="M84" t="s">
@@ -4315,7 +4213,7 @@
         <v>20</v>
       </c>
       <c r="O84" s="1">
-        <f t="shared" ref="O84:O87" si="33">N84*($B$81/100)</f>
+        <f t="shared" ref="O84:O87" si="39">N84*($B$81/100)</f>
         <v>1</v>
       </c>
       <c r="Q84" t="s">
@@ -4325,7 +4223,7 @@
         <v>5</v>
       </c>
       <c r="S84" s="1">
-        <f t="shared" ref="S84:S87" si="34">R84*($B$81/100)</f>
+        <f t="shared" ref="S84:S87" si="40">R84*($B$81/100)</f>
         <v>0.25</v>
       </c>
       <c r="U84" t="s">
@@ -4335,115 +4233,91 @@
         <v>5</v>
       </c>
       <c r="W84" s="1">
-        <f t="shared" ref="W84:W87" si="35">V84*($B$81/100)</f>
+        <f t="shared" ref="W84:W87" si="41">V84*($B$81/100)</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85">
-        <v>2</v>
-      </c>
       <c r="C85" s="1">
-        <f t="shared" si="30"/>
-        <v>0.1</v>
-      </c>
-      <c r="E85" t="s">
-        <v>27</v>
-      </c>
-      <c r="F85">
-        <v>10</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
       <c r="G85" s="1">
-        <f t="shared" si="31"/>
-        <v>0.5</v>
+        <f t="shared" si="37"/>
+        <v>0</v>
       </c>
       <c r="K85" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O85" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="S85" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W85" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="A86" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="30"/>
-        <v>0.1</v>
-      </c>
-      <c r="E86" t="s">
-        <v>85</v>
-      </c>
-      <c r="F86">
-        <v>5</v>
+        <f t="shared" si="36"/>
+        <v>1.25</v>
       </c>
       <c r="G86" s="1">
-        <f t="shared" si="31"/>
-        <v>0.25</v>
+        <f t="shared" si="37"/>
+        <v>0</v>
       </c>
       <c r="K86" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O86" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="S86" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W86" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>81</v>
-      </c>
-      <c r="B87">
-        <v>2</v>
-      </c>
       <c r="C87" s="1">
-        <f t="shared" si="30"/>
-        <v>0.1</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
       <c r="G87" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K87" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O87" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="S87" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W87" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
     </row>
@@ -4471,6 +4345,11 @@
       <c r="U88" s="12"/>
       <c r="V88" s="12"/>
       <c r="W88" s="12"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B22 F22 J22 N22 R22 V22 B35 F35 J35 N35 R35 V35 B64 F64 J64 N64 R64 V64 B73 F73 J73 N73 R73 V73 B82 F82 J82 N82 R82 V82">
@@ -4523,7 +4402,7 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5799,7 +5678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D437AB-C2CB-8D43-BD8D-11D3278E662B}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>

</xml_diff>